<commit_message>
Cambio tamaño de imágenes
Por cambio de motor (se quita f13)
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC160.xlsx
+++ b/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC160.xlsx
@@ -16,12 +16,12 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="205">
   <si>
     <t>Fecha:</t>
   </si>
@@ -603,31 +603,40 @@
     <t>Modificar en la imagen los textos: Normal Blood Vessel por Vaso Sanguineo Normal; Hamorrhage por Hemorragia; Clotting por Coagulación; Healthy por Saludable; Inability to Clot por Incapaz de Coagular; Haemophilia por Hemofilia.</t>
   </si>
   <si>
-    <t>Niño usando inhalados para asma.</t>
-  </si>
-  <si>
-    <t>Pareja de abuelos</t>
-  </si>
-  <si>
     <t>Pareja con síndrome de Down en trineo</t>
   </si>
   <si>
-    <t>Examen de epilepsia</t>
-  </si>
-  <si>
     <t>Diagrama de la fibrosis quística</t>
   </si>
   <si>
     <t>Modificar en la imagen los textos: Trachea por Traquea, Lung por Pulmón, Smoot muscle por Músculo liso, Tracheas muscle por Músculo traqueal, Inflammatios por Inflamación, Increased mucus secretion por Incremanta la secreción de moco, Thickened smooth muscle por Músculo liso engrosado, Narrow lumen por Lumen estrecho, Healthy por Saludable, Cystic Fibrosis por Fibrosis Cística.</t>
   </si>
   <si>
-    <t>Mujer con pañoleta en la cabeza representando una paciente con cáncer</t>
-  </si>
-  <si>
     <t>Cromosoma con ADN visible en su interior</t>
   </si>
   <si>
     <t>Ajustar la imagen para que sea notorio que uno de los extremos del cromosoma está roto y ha desaparecido.</t>
+  </si>
+  <si>
+    <t>Niño usando inhalador para asma.</t>
+  </si>
+  <si>
+    <t>Ilustración</t>
+  </si>
+  <si>
+    <t>Una cadena de ADN</t>
+  </si>
+  <si>
+    <t>Varias cadenas de ADN</t>
+  </si>
+  <si>
+    <t>Mitocondria</t>
+  </si>
+  <si>
+    <t>Óvulos y espermatozoides</t>
+  </si>
+  <si>
+    <t>Mujer pinchándose un dedo</t>
   </si>
 </sst>
 </file>
@@ -2405,9 +2414,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K101" sqref="K101"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2454,7 @@
       </c>
       <c r="M1" s="2" t="str">
         <f>CONCATENATE('Definición técnica de imagenes'!$B$1," ",$G$5)</f>
-        <v>Ubicación de la imagen en el recurso F13</v>
+        <v>Ubicación de la imagen en el recurso F6</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2469,7 +2478,7 @@
       </c>
       <c r="M2" s="2" t="str">
         <f ca="1">IF($N2&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N2,1,1,1),"")</f>
-        <v>Simple</v>
+        <v>Inicio</v>
       </c>
       <c r="N2" s="2">
         <v>0</v>
@@ -2500,7 +2509,7 @@
       </c>
       <c r="M3" s="2" t="str">
         <f ca="1">IF($N3&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N3,1,1,1),"")</f>
-        <v>Doble</v>
+        <v>Contenido</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -2557,7 +2566,7 @@
         <v>Motor del recurso</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
@@ -2670,7 +2679,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>IF($G$4="Recurso",$M$1,$L$1)</f>
-        <v>Ubicación de la imagen en el recurso F13</v>
+        <v>Ubicación de la imagen en el recurso F6</v>
       </c>
       <c r="F9" s="57" t="s">
         <v>61</v>
@@ -2695,46 +2704,44 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="108" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62">
-        <v>298069352</v>
+        <v>236181712</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D10" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_07_REC160_IMG01n.jpg</v>
+        <v>CN_08_07_REC160_IMG01.jpg</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>350 x 230 px</v>
       </c>
       <c r="H10" s="13" t="str">
         <f t="shared" ref="H10" ca="1" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>CN_08_07_REC160_IMG01a.jpg</v>
+        <v/>
       </c>
       <c r="I10" s="13" t="str">
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="K10" s="64" t="s">
-        <v>192</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
@@ -2746,17 +2753,17 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62">
-        <v>299798345</v>
+        <v>298069352</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2764,7 +2771,7 @@
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>320 x 480 px</v>
       </c>
       <c r="H11" s="13" t="str">
         <f t="shared" ref="H11:H74" ca="1" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
@@ -2772,12 +2779,14 @@
       </c>
       <c r="I11" s="13" t="str">
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>800 x 458 px</v>
       </c>
       <c r="J11" s="64" t="s">
-        <v>193</v>
-      </c>
-      <c r="K11" s="65"/>
+        <v>191</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>192</v>
+      </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
         <v>M101</v>
@@ -2789,36 +2798,36 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="62">
-        <v>194770151</v>
+        <v>116931397</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_07_REC160_IMG03n.jpg</v>
+        <v>CN_08_07_REC160_IMG03.jpg</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>350 x 230 px</v>
       </c>
       <c r="H12" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_07_REC160_IMG03a.jpg</v>
+        <v/>
       </c>
       <c r="I12" s="13" t="str">
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J12" s="64" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -2832,17 +2841,17 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62">
-        <v>61676032</v>
+        <v>299798345</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D13" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2850,7 +2859,7 @@
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>320 x 480 px</v>
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2858,10 +2867,10 @@
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>800 x 458 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
@@ -2879,35 +2888,35 @@
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_07_REC160_IMG05n.jpg</v>
+        <v>CN_08_07_REC160_IMG05.jpg</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>350 x 230 px</v>
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_07_REC160_IMG05a.jpg</v>
+        <v/>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J14" s="64" t="s">
-        <v>200</v>
-      </c>
-      <c r="K14" s="64" t="s">
-        <v>201</v>
+        <v/>
+      </c>
+      <c r="J14" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>197</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
@@ -2920,17 +2929,17 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62">
-        <v>13397869</v>
+        <v>61676032</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D15" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2938,7 +2947,7 @@
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 375 px</v>
+        <v>320 x 480 px</v>
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2946,79 +2955,77 @@
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="K15" s="66"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J15" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="K15" s="64"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="175.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
       <c r="B16" s="62">
-        <v>203333557</v>
+        <v>72239452</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D16" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_07_REC160_IMG07n.jpg</v>
+        <v>CN_08_07_REC160_IMG07.jpg</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>350 x 230 px</v>
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_07_REC160_IMG07a.jpg</v>
+        <v/>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v/>
       </c>
       <c r="J16" s="67" t="s">
-        <v>197</v>
-      </c>
-      <c r="K16" s="64" t="s">
-        <v>198</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="K16" s="64"/>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="175.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
       <c r="B17" s="62">
-        <v>163011854</v>
+        <v>203333557</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F13</v>
+        <v>Recurso F6</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E17" s="63" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F17" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -3026,7 +3033,7 @@
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>240 x 185 px</v>
+        <v>320 x 480 px</v>
       </c>
       <c r="H17" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3034,12 +3041,14 @@
       </c>
       <c r="I17" s="13" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 460 px</v>
+        <v>800 x 458 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>199</v>
-      </c>
-      <c r="K17" s="66"/>
+        <v>194</v>
+      </c>
+      <c r="K17" s="66" t="s">
+        <v>195</v>
+      </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
         <v>F7B</v>
@@ -3048,22 +3057,28 @@
     <row r="18" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B18" s="62"/>
+        <v>IMG09</v>
+      </c>
+      <c r="B18" s="62">
+        <v>251869774</v>
+      </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>150</v>
+      </c>
       <c r="F18" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>CN_08_07_REC160_IMG09.jpg</v>
       </c>
       <c r="G18" s="13" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>350 x 230 px</v>
       </c>
       <c r="H18" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3073,7 +3088,9 @@
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J18" s="66"/>
+      <c r="J18" s="66" t="s">
+        <v>203</v>
+      </c>
       <c r="K18" s="66"/>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3083,32 +3100,40 @@
     <row r="19" spans="1:15" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
-        <v/>
-      </c>
-      <c r="B19" s="62"/>
+        <v>IMG10</v>
+      </c>
+      <c r="B19" s="62">
+        <v>299694263</v>
+      </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
+        <v>Recurso F6</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>155</v>
+      </c>
       <c r="F19" s="13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" ca="1" si="4"/>
+        <v>CN_08_07_REC160_IMG10n.jpg</v>
       </c>
       <c r="G19" s="13" t="str">
         <f ca="1">IF($F19&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
+        <v>320 x 480 px</v>
       </c>
       <c r="H19" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>CN_08_07_REC160_IMG10a.jpg</v>
       </c>
       <c r="I19" s="13" t="str">
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v/>
-      </c>
-      <c r="J19" s="67"/>
+        <v>800 x 458 px</v>
+      </c>
+      <c r="J19" s="67" t="s">
+        <v>204</v>
+      </c>
       <c r="K19" s="68"/>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>

</xml_diff>